<commit_message>
Save in a file all the changes
</commit_message>
<xml_diff>
--- a/vehiculos_info.xlsx
+++ b/vehiculos_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siste\Documents\git_repos\adeudo-vehicular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3660A5E1-0195-4DF1-A001-8C70B3B3E35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EEA655-FCE9-451A-9286-EA7D8B23242C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0D5B64AA-EC10-40C1-90C7-C99B1029935E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0D5B64AA-EC10-40C1-90C7-C99B1029935E}"/>
   </bookViews>
   <sheets>
     <sheet name="informacion_vehicular" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
   <si>
     <t>camioneta</t>
   </si>
@@ -56,27 +56,6 @@
     <t>n/ serie del motor</t>
   </si>
   <si>
-    <t>JW06845</t>
-  </si>
-  <si>
-    <t>3GBJC34R55M120648</t>
-  </si>
-  <si>
-    <t>H EN M</t>
-  </si>
-  <si>
-    <t>D21</t>
-  </si>
-  <si>
-    <t>JW32486</t>
-  </si>
-  <si>
-    <t>3N6CD15SXYK049323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KA24881160M </t>
-  </si>
-  <si>
     <t>NP300</t>
   </si>
   <si>
@@ -89,30 +68,6 @@
     <t>KA24536833A</t>
   </si>
   <si>
-    <t>JV09589</t>
-  </si>
-  <si>
-    <t>3N6DD25T69K035827</t>
-  </si>
-  <si>
-    <t>KA24424370A</t>
-  </si>
-  <si>
-    <t>JW06814</t>
-  </si>
-  <si>
-    <t>3N6CD15S74K128278</t>
-  </si>
-  <si>
-    <t>KA24184506A</t>
-  </si>
-  <si>
-    <t>JV90444</t>
-  </si>
-  <si>
-    <t>3GBJC34R56M117914</t>
-  </si>
-  <si>
     <t>JS14993</t>
   </si>
   <si>
@@ -158,9 +113,6 @@
     <t>KA24616699A</t>
   </si>
   <si>
-    <t>JX13960</t>
-  </si>
-  <si>
     <t>3N6DD25T4AK014852</t>
   </si>
   <si>
@@ -288,16 +240,55 @@
   </si>
   <si>
     <t>KA24855277A</t>
+  </si>
+  <si>
+    <t>JY63903</t>
+  </si>
+  <si>
+    <t>3N6AD35A0RK812266</t>
+  </si>
+  <si>
+    <t>QR25549396H</t>
+  </si>
+  <si>
+    <t>NOMBRE PROPIETARIO</t>
+  </si>
+  <si>
+    <t>CARLOS SANTANA RUELAS</t>
+  </si>
+  <si>
+    <t>ACTIVOS PRODUCTIVOS SA DE CV</t>
+  </si>
+  <si>
+    <t>JY53291</t>
+  </si>
+  <si>
+    <t>JAC</t>
+  </si>
+  <si>
+    <t>JY63933</t>
+  </si>
+  <si>
+    <t>3GAPJ1A90SM016075</t>
+  </si>
+  <si>
+    <t>R4406476</t>
+  </si>
+  <si>
+    <t>JY63934</t>
+  </si>
+  <si>
+    <t>3GAPJ1A94SM016077</t>
+  </si>
+  <si>
+    <t>R4406478</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,13 +301,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -333,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -356,12 +340,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -374,10 +368,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -710,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23532B29-6155-423B-BB67-0D2AAB9E0580}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,10 +716,11 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,36 +739,42 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G1" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>3500</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="5">
-        <v>2005</v>
+        <v>2012</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="5">
-        <v>2000</v>
+        <v>2011</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>10</v>
@@ -784,194 +785,223 @@
       <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G3" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2014</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5">
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2014</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2015</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2013</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2010</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5">
         <v>2012</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="D9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="5">
-        <v>2009</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2004</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4">
-        <v>3500</v>
-      </c>
-      <c r="C7" s="5">
-        <v>2006</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5">
-        <v>2011</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5">
-        <v>2014</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C10" s="5">
         <v>2014</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G10" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C11" s="5">
         <v>2015</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2014</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>15</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="5">
-        <v>2013</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>16</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C13" s="5">
         <v>2010</v>
@@ -985,225 +1015,215 @@
       <c r="F13" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G13" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C14" s="5">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2015</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2024</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>25</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="5">
+        <v>2024</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>26</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2024</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="C19" s="5">
+        <v>2019</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>18</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="5">
-        <v>2014</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="G19" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="5">
+        <v>2019</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>19</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="5">
-        <v>2015</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="G20" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="C21" s="5">
+        <v>2016</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>20</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="5">
-        <v>2014</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G21" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>21</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="C22" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="5">
-        <v>2010</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>22</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="5">
-        <v>2013</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>23</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="5">
-        <v>2015</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="5">
-        <v>2019</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="5">
-        <v>2019</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="5">
-        <v>2016</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="5">
-        <v>2018</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>73</v>
+      <c r="G22" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>